<commit_message>
Updated with error handling around sheet name change
</commit_message>
<xml_diff>
--- a/uploads/123-upload-2018-02-15.xlsx
+++ b/uploads/123-upload-2018-02-15.xlsx
@@ -1,30 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10214"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laptop\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ephillips/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43820" yWindow="-7820" windowWidth="29540" windowHeight="17120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DMA" sheetId="1" r:id="rId1"/>
+    <sheet name="DMA - January" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Tactic</t>
   </si>
   <si>
-    <t>0162</t>
+    <t>1438</t>
+  </si>
+  <si>
+    <t>0970</t>
+  </si>
+  <si>
+    <t>0934</t>
+  </si>
+  <si>
+    <t>0675</t>
   </si>
   <si>
     <t>Television</t>
@@ -104,15 +118,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="\$0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,15 +153,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -478,217 +499,517 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="DMA"/>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.796875" customWidth="1"/>
-    <col min="2" max="2" width="10.69921875" customWidth="1"/>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>2242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>13392</v>
+      </c>
+      <c r="C6" s="1">
+        <v>13392</v>
+      </c>
+      <c r="D6" s="1">
+        <v>13392</v>
+      </c>
+      <c r="E6" s="1">
+        <v>13392</v>
+      </c>
+      <c r="F6" s="1">
+        <v>13392</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>7568</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7531</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7643</v>
+      </c>
+      <c r="E7" s="1">
+        <v>7334</v>
+      </c>
+      <c r="F7" s="1">
+        <v>7436</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>646</v>
+      </c>
+      <c r="C10" s="1">
+        <v>646</v>
+      </c>
+      <c r="D10" s="1">
+        <v>646</v>
+      </c>
+      <c r="E10" s="1">
+        <v>646</v>
+      </c>
+      <c r="F10" s="1">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1413</v>
+      </c>
+      <c r="C11" s="1">
+        <f>1100+1300</f>
+        <v>2400</v>
+      </c>
+      <c r="D11" s="1">
+        <f>2900+1300</f>
+        <v>4200</v>
+      </c>
+      <c r="E11" s="1">
+        <f>1100+1300</f>
+        <v>2400</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>2314</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2314</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2314</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2314</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C14" s="1">
+        <v>1200</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>9403</v>
+      </c>
+      <c r="C22" s="1">
+        <v>24421</v>
+      </c>
+      <c r="D22" s="1">
+        <v>27632</v>
+      </c>
+      <c r="E22" s="1">
+        <v>15568</v>
+      </c>
+      <c r="F22" s="1">
+        <v>22343</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1">
         <f t="array" ref="B23">SUM(B2:B22)</f>
-        <v>11200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>35086</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="array" ref="C23">SUM(C2:C22)</f>
+        <v>51904</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="array" ref="D23">SUM(D2:D22)</f>
+        <v>55827</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="array" ref="E23">SUM(E2:E22)</f>
+        <v>41654</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="array" ref="F23">SUM(F2:F22)</f>
+        <v>48931</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
       </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>